<commit_message>
commit para checkout a codigo
</commit_message>
<xml_diff>
--- a/resultados/excels/banco dc 06-05-2022.xlsx
+++ b/resultados/excels/banco dc 06-05-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPM\4 - Cuarto\TFG\Datum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPM\4 - Cuarto\TFG\Repo\TFG-Mano-amiga\resultados\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C81952-EA41-47B7-BB5E-30BA152056A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439E719F-4193-41FD-89D9-6013A9E19168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1" sheetId="1" r:id="rId1"/>
@@ -799,62 +799,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>Sin sat. subidas</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1130,6 +1075,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Intensidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> (mA)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1192,6 +1197,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Fuerza</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> (g)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2943,67 +3008,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>Sin sat,</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-ES" baseline="0"/>
-              <a:t> bajadas</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-ES"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -3050,8 +3055,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.3402594050743657"/>
-                  <c:y val="8.8425925925925929E-3"/>
+                  <c:x val="-0.44581496062992126"/>
+                  <c:y val="0.12425634295713035"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -3183,6 +3188,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Intensidad (mA)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3245,6 +3305,64 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Fuerza (g)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3352,62 +3470,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>Todo</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -3837,6 +3900,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Intensidad (mA)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3899,6 +4017,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Fuerza (g)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -16872,8 +17045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903E4D83-D2B3-4DD7-8827-6BC325CCFB06}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16907,15 +17080,15 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <f>B3-B2</f>
+        <f t="shared" ref="D2:D33" si="0">B3-B2</f>
         <v>2</v>
       </c>
       <c r="E2">
-        <f>A3-A2</f>
+        <f t="shared" ref="E2:E33" si="1">A3-A2</f>
         <v>13</v>
       </c>
       <c r="F2">
-        <f>D2/E2</f>
+        <f t="shared" ref="F2:F33" si="2">D2/E2</f>
         <v>0.15384615384615385</v>
       </c>
     </row>
@@ -16927,15 +17100,15 @@
         <v>34.799999999999997</v>
       </c>
       <c r="D3">
-        <f>B4-B3</f>
+        <f t="shared" si="0"/>
         <v>1.4000000000000057</v>
       </c>
       <c r="E3">
-        <f>A4-A3</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F3">
-        <f>D3/E3</f>
+        <f t="shared" si="2"/>
         <v>0.35000000000000142</v>
       </c>
     </row>
@@ -16947,15 +17120,15 @@
         <v>36.200000000000003</v>
       </c>
       <c r="D4">
-        <f>B5-B4</f>
+        <f t="shared" si="0"/>
         <v>1.8999999999999986</v>
       </c>
       <c r="E4">
-        <f>A5-A4</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F4">
-        <f>D4/E4</f>
+        <f t="shared" si="2"/>
         <v>0.47499999999999964</v>
       </c>
     </row>
@@ -16967,15 +17140,15 @@
         <v>38.1</v>
       </c>
       <c r="D5">
-        <f>B6-B5</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="E5">
-        <f>A6-A5</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="F5">
-        <f>D5/E5</f>
+        <f t="shared" si="2"/>
         <v>0.27777777777777779</v>
       </c>
     </row>
@@ -16987,15 +17160,15 @@
         <v>40.6</v>
       </c>
       <c r="D6">
-        <f>B7-B6</f>
+        <f t="shared" si="0"/>
         <v>4.3999999999999986</v>
       </c>
       <c r="E6">
-        <f>A7-A6</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="F6">
-        <f>D6/E6</f>
+        <f t="shared" si="2"/>
         <v>0.36666666666666653</v>
       </c>
     </row>
@@ -17007,15 +17180,15 @@
         <v>45</v>
       </c>
       <c r="D7">
-        <f>B8-B7</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E7">
-        <f>A8-A7</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F7">
-        <f>D7/E7</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
@@ -17027,15 +17200,15 @@
         <v>49</v>
       </c>
       <c r="D8">
-        <f>B9-B8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E8">
-        <f>A9-A8</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="F8">
-        <f>D8/E8</f>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
     </row>
@@ -17047,15 +17220,15 @@
         <v>50</v>
       </c>
       <c r="D9">
-        <f>B10-B9</f>
+        <f t="shared" si="0"/>
         <v>4.7000000000000028</v>
       </c>
       <c r="E9">
-        <f>A10-A9</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="F9">
-        <f>D9/E9</f>
+        <f t="shared" si="2"/>
         <v>0.39166666666666689</v>
       </c>
     </row>
@@ -17067,15 +17240,15 @@
         <v>54.7</v>
       </c>
       <c r="D10">
-        <f>B11-B10</f>
+        <f t="shared" si="0"/>
         <v>3.8999999999999986</v>
       </c>
       <c r="E10">
-        <f>A11-A10</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F10">
-        <f>D10/E10</f>
+        <f t="shared" si="2"/>
         <v>0.55714285714285694</v>
       </c>
     </row>
@@ -17087,15 +17260,15 @@
         <v>58.6</v>
       </c>
       <c r="D11">
-        <f>B12-B11</f>
+        <f t="shared" si="0"/>
         <v>3.8999999999999986</v>
       </c>
       <c r="E11">
-        <f>A12-A11</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F11">
-        <f>D11/E11</f>
+        <f t="shared" si="2"/>
         <v>0.55714285714285694</v>
       </c>
     </row>
@@ -17107,15 +17280,15 @@
         <v>62.5</v>
       </c>
       <c r="D12">
-        <f>B13-B12</f>
+        <f t="shared" si="0"/>
         <v>5.9000000000000057</v>
       </c>
       <c r="E12">
-        <f>A13-A12</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="F12">
-        <f>D12/E12</f>
+        <f t="shared" si="2"/>
         <v>0.42142857142857182</v>
       </c>
     </row>
@@ -17127,15 +17300,15 @@
         <v>68.400000000000006</v>
       </c>
       <c r="D13">
-        <f>B14-B13</f>
+        <f t="shared" si="0"/>
         <v>1.2999999999999972</v>
       </c>
       <c r="E13">
-        <f>A14-A13</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F13">
-        <f>D13/E13</f>
+        <f t="shared" si="2"/>
         <v>0.12999999999999973</v>
       </c>
     </row>
@@ -17147,15 +17320,15 @@
         <v>69.7</v>
       </c>
       <c r="D14">
-        <f>B15-B14</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="E14">
-        <f>A15-A14</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="F14">
-        <f>D14/E14</f>
+        <f t="shared" si="2"/>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -17170,15 +17343,15 @@
         <v>7</v>
       </c>
       <c r="D15">
-        <f>B16-B15</f>
+        <f t="shared" si="0"/>
         <v>-0.20000000000000284</v>
       </c>
       <c r="E15">
-        <f>A16-A15</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F15">
-        <f>D15/E15</f>
+        <f t="shared" si="2"/>
         <v>-1.8181818181818441E-2</v>
       </c>
     </row>
@@ -17190,15 +17363,15 @@
         <v>70</v>
       </c>
       <c r="D16">
-        <f>B17-B16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E16">
-        <f>A17-A16</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F16">
-        <f>D16/E16</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -17210,15 +17383,15 @@
         <v>70</v>
       </c>
       <c r="D17">
-        <f>B18-B17</f>
+        <f t="shared" si="0"/>
         <v>-6</v>
       </c>
       <c r="E17">
-        <f>A18-A17</f>
+        <f t="shared" si="1"/>
         <v>-106</v>
       </c>
       <c r="F17">
-        <f>D17/E17</f>
+        <f t="shared" si="2"/>
         <v>5.6603773584905662E-2</v>
       </c>
     </row>
@@ -17233,15 +17406,15 @@
         <v>8</v>
       </c>
       <c r="D18">
-        <f>B19-B18</f>
+        <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
       <c r="E18">
-        <f>A19-A18</f>
+        <f t="shared" si="1"/>
         <v>-6</v>
       </c>
       <c r="F18">
-        <f>D18/E18</f>
+        <f t="shared" si="2"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
@@ -17253,15 +17426,15 @@
         <v>63.5</v>
       </c>
       <c r="D19">
-        <f>B20-B19</f>
+        <f t="shared" si="0"/>
         <v>-18.299999999999997</v>
       </c>
       <c r="E19">
-        <f>A20-A19</f>
+        <f t="shared" si="1"/>
         <v>-12</v>
       </c>
       <c r="F19">
-        <f>D19/E19</f>
+        <f t="shared" si="2"/>
         <v>1.5249999999999997</v>
       </c>
     </row>
@@ -17273,15 +17446,15 @@
         <v>45.2</v>
       </c>
       <c r="D20">
-        <f>B21-B20</f>
+        <f t="shared" si="0"/>
         <v>-3.5</v>
       </c>
       <c r="E20">
-        <f>A21-A20</f>
+        <f t="shared" si="1"/>
         <v>-10</v>
       </c>
       <c r="F20">
-        <f>D20/E20</f>
+        <f t="shared" si="2"/>
         <v>0.35</v>
       </c>
     </row>
@@ -17293,15 +17466,15 @@
         <v>41.7</v>
       </c>
       <c r="D21">
-        <f>B22-B21</f>
+        <f t="shared" si="0"/>
         <v>-6.2000000000000028</v>
       </c>
       <c r="E21">
-        <f>A22-A21</f>
+        <f t="shared" si="1"/>
         <v>-15</v>
       </c>
       <c r="F21">
-        <f>D21/E21</f>
+        <f t="shared" si="2"/>
         <v>0.4133333333333335</v>
       </c>
     </row>
@@ -17313,15 +17486,15 @@
         <v>35.5</v>
       </c>
       <c r="D22">
-        <f>B23-B22</f>
+        <f t="shared" si="0"/>
         <v>-5.3999999999999986</v>
       </c>
       <c r="E22">
-        <f>A23-A22</f>
+        <f t="shared" si="1"/>
         <v>-13</v>
       </c>
       <c r="F22">
-        <f>D22/E22</f>
+        <f t="shared" si="2"/>
         <v>0.4153846153846153</v>
       </c>
     </row>
@@ -17333,15 +17506,15 @@
         <v>30.1</v>
       </c>
       <c r="D23">
-        <f>B24-B23</f>
+        <f t="shared" si="0"/>
         <v>-3.1000000000000014</v>
       </c>
       <c r="E23">
-        <f>A24-A23</f>
+        <f t="shared" si="1"/>
         <v>-11</v>
       </c>
       <c r="F23">
-        <f>D23/E23</f>
+        <f t="shared" si="2"/>
         <v>0.28181818181818197</v>
       </c>
     </row>
@@ -17356,15 +17529,15 @@
         <v>7</v>
       </c>
       <c r="D24">
-        <f>B25-B24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E24">
-        <f>A25-A24</f>
+        <f t="shared" si="1"/>
         <v>-6</v>
       </c>
       <c r="F24">
-        <f>D24/E24</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -17376,15 +17549,15 @@
         <v>27</v>
       </c>
       <c r="D25">
-        <f>B26-B25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E25">
-        <f>A26-A25</f>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="F25">
-        <f>D25/E25</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -17396,15 +17569,15 @@
         <v>27</v>
       </c>
       <c r="D26">
-        <f>B27-B26</f>
+        <f t="shared" si="0"/>
         <v>0.30000000000000071</v>
       </c>
       <c r="E26">
-        <f>A27-A26</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F26">
-        <f>D26/E26</f>
+        <f t="shared" si="2"/>
         <v>5.0000000000000121E-2</v>
       </c>
     </row>
@@ -17419,15 +17592,15 @@
         <v>9</v>
       </c>
       <c r="D27">
-        <f>B28-B27</f>
+        <f t="shared" si="0"/>
         <v>-0.10000000000000142</v>
       </c>
       <c r="E27">
-        <f>A28-A27</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F27">
-        <f>D27/E27</f>
+        <f t="shared" si="2"/>
         <v>-1.4285714285714488E-2</v>
       </c>
     </row>
@@ -17439,15 +17612,15 @@
         <v>27.2</v>
       </c>
       <c r="D28">
-        <f>B29-B28</f>
+        <f t="shared" si="0"/>
         <v>1.3000000000000007</v>
       </c>
       <c r="E28">
-        <f>A29-A28</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="F28">
-        <f>D28/E28</f>
+        <f t="shared" si="2"/>
         <v>5.4166666666666696E-2</v>
       </c>
     </row>
@@ -17459,15 +17632,15 @@
         <v>28.5</v>
       </c>
       <c r="D29">
-        <f>B30-B29</f>
+        <f t="shared" si="0"/>
         <v>2.1000000000000014</v>
       </c>
       <c r="E29">
-        <f>A30-A29</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F29">
-        <f>D29/E29</f>
+        <f t="shared" si="2"/>
         <v>0.21000000000000013</v>
       </c>
     </row>
@@ -17479,15 +17652,15 @@
         <v>30.6</v>
       </c>
       <c r="D30">
-        <f>B31-B30</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E30">
-        <f>A31-A30</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="F30">
-        <f>D30/E30</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -17499,15 +17672,15 @@
         <v>33.6</v>
       </c>
       <c r="D31">
-        <f>B32-B31</f>
+        <f t="shared" si="0"/>
         <v>6.8999999999999986</v>
       </c>
       <c r="E31">
-        <f>A32-A31</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="F31">
-        <f>D31/E31</f>
+        <f t="shared" si="2"/>
         <v>0.40588235294117636</v>
       </c>
     </row>
@@ -17519,15 +17692,15 @@
         <v>40.5</v>
       </c>
       <c r="D32">
-        <f>B33-B32</f>
+        <f t="shared" si="0"/>
         <v>4.1000000000000014</v>
       </c>
       <c r="E32">
-        <f>A33-A32</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F32">
-        <f>D32/E32</f>
+        <f t="shared" si="2"/>
         <v>0.41000000000000014</v>
       </c>
     </row>
@@ -17539,15 +17712,15 @@
         <v>44.6</v>
       </c>
       <c r="D33">
-        <f>B34-B33</f>
+        <f t="shared" si="0"/>
         <v>5.1000000000000014</v>
       </c>
       <c r="E33">
-        <f>A34-A33</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="F33">
-        <f>D33/E33</f>
+        <f t="shared" si="2"/>
         <v>0.36428571428571438</v>
       </c>
     </row>
@@ -17559,15 +17732,15 @@
         <v>49.7</v>
       </c>
       <c r="D34">
-        <f>B35-B34</f>
+        <f t="shared" ref="D34:D57" si="3">B35-B34</f>
         <v>6.2999999999999972</v>
       </c>
       <c r="E34">
-        <f>A35-A34</f>
+        <f t="shared" ref="E34:E57" si="4">A35-A34</f>
         <v>8</v>
       </c>
       <c r="F34">
-        <f>D34/E34</f>
+        <f t="shared" ref="F34:F65" si="5">D34/E34</f>
         <v>0.78749999999999964</v>
       </c>
     </row>
@@ -17579,15 +17752,15 @@
         <v>56</v>
       </c>
       <c r="D35">
-        <f>B36-B35</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="E35">
-        <f>A36-A35</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="F35">
-        <f>D35/E35</f>
+        <f t="shared" si="5"/>
         <v>0.53333333333333333</v>
       </c>
     </row>
@@ -17599,15 +17772,15 @@
         <v>64</v>
       </c>
       <c r="D36">
-        <f>B37-B36</f>
+        <f t="shared" si="3"/>
         <v>-0.5</v>
       </c>
       <c r="E36">
-        <f>A37-A36</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="F36">
-        <f>D36/E36</f>
+        <f t="shared" si="5"/>
         <v>-0.1</v>
       </c>
     </row>
@@ -17619,15 +17792,15 @@
         <v>63.5</v>
       </c>
       <c r="D37">
-        <f>B38-B37</f>
+        <f t="shared" si="3"/>
         <v>3.5</v>
       </c>
       <c r="E37">
-        <f>A38-A37</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="F37">
-        <f>D37/E37</f>
+        <f t="shared" si="5"/>
         <v>0.23333333333333334</v>
       </c>
     </row>
@@ -17639,15 +17812,15 @@
         <v>67</v>
       </c>
       <c r="D38">
-        <f>B39-B38</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E38">
-        <f>A39-A38</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="F38">
-        <f>D38/E38</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -17659,15 +17832,15 @@
         <v>67</v>
       </c>
       <c r="D39">
-        <f>B40-B39</f>
+        <f t="shared" si="3"/>
         <v>1.2999999999999972</v>
       </c>
       <c r="E39">
-        <f>A40-A39</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="F39">
-        <f>D39/E39</f>
+        <f t="shared" si="5"/>
         <v>5.1999999999999887E-2</v>
       </c>
     </row>
@@ -17679,15 +17852,15 @@
         <v>68.3</v>
       </c>
       <c r="D40">
-        <f>B41-B40</f>
+        <f t="shared" si="3"/>
         <v>3.2999999999999972</v>
       </c>
       <c r="E40">
-        <f>A41-A40</f>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="F40">
-        <f>D40/E40</f>
+        <f t="shared" si="5"/>
         <v>7.0212765957446743E-2</v>
       </c>
     </row>
@@ -17702,15 +17875,15 @@
         <v>7</v>
       </c>
       <c r="D41">
-        <f>B42-B41</f>
+        <f t="shared" si="3"/>
         <v>-9.9999999999994316E-2</v>
       </c>
       <c r="E41">
-        <f>A42-A41</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="F41">
-        <f>D41/E41</f>
+        <f t="shared" si="5"/>
         <v>-2.8571428571426949E-3</v>
       </c>
     </row>
@@ -17722,15 +17895,15 @@
         <v>71.5</v>
       </c>
       <c r="D42">
-        <f>B43-B42</f>
+        <f t="shared" si="3"/>
         <v>-0.5</v>
       </c>
       <c r="E42">
-        <f>A43-A42</f>
+        <f t="shared" si="4"/>
         <v>-72</v>
       </c>
       <c r="F42">
-        <f>D42/E42</f>
+        <f t="shared" si="5"/>
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
@@ -17745,15 +17918,15 @@
         <v>8</v>
       </c>
       <c r="D43">
-        <f>B44-B43</f>
+        <f t="shared" si="3"/>
         <v>-0.59999999999999432</v>
       </c>
       <c r="E43">
-        <f>A44-A43</f>
+        <f t="shared" si="4"/>
         <v>-17</v>
       </c>
       <c r="F43">
-        <f>D43/E43</f>
+        <f t="shared" si="5"/>
         <v>3.529411764705849E-2</v>
       </c>
     </row>
@@ -17765,15 +17938,15 @@
         <v>70.400000000000006</v>
       </c>
       <c r="D44">
-        <f>B45-B44</f>
+        <f t="shared" si="3"/>
         <v>-0.90000000000000568</v>
       </c>
       <c r="E44">
-        <f>A45-A44</f>
+        <f t="shared" si="4"/>
         <v>-25</v>
       </c>
       <c r="F44">
-        <f>D44/E44</f>
+        <f t="shared" si="5"/>
         <v>3.6000000000000226E-2</v>
       </c>
     </row>
@@ -17785,15 +17958,15 @@
         <v>69.5</v>
       </c>
       <c r="D45">
-        <f>B46-B45</f>
+        <f t="shared" si="3"/>
         <v>-0.20000000000000284</v>
       </c>
       <c r="E45">
-        <f>A46-A45</f>
+        <f t="shared" si="4"/>
         <v>-11</v>
       </c>
       <c r="F45">
-        <f>D45/E45</f>
+        <f t="shared" si="5"/>
         <v>1.8181818181818441E-2</v>
       </c>
     </row>
@@ -17805,15 +17978,15 @@
         <v>69.3</v>
       </c>
       <c r="D46">
-        <f>B47-B46</f>
+        <f t="shared" si="3"/>
         <v>-1.7000000000000028</v>
       </c>
       <c r="E46">
-        <f>A47-A46</f>
+        <f t="shared" si="4"/>
         <v>-19</v>
       </c>
       <c r="F46">
-        <f>D46/E46</f>
+        <f t="shared" si="5"/>
         <v>8.9473684210526469E-2</v>
       </c>
     </row>
@@ -17825,15 +17998,15 @@
         <v>67.599999999999994</v>
       </c>
       <c r="D47">
-        <f>B48-B47</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E47">
-        <f>A48-A47</f>
+        <f t="shared" si="4"/>
         <v>-8</v>
       </c>
       <c r="F47">
-        <f>D47/E47</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -17845,15 +18018,15 @@
         <v>67.599999999999994</v>
       </c>
       <c r="D48">
-        <f>B49-B48</f>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="E48">
-        <f>A49-A48</f>
+        <f t="shared" si="4"/>
         <v>-16</v>
       </c>
       <c r="F48">
-        <f>D48/E48</f>
+        <f t="shared" si="5"/>
         <v>0.1875</v>
       </c>
     </row>
@@ -17865,15 +18038,15 @@
         <v>64.599999999999994</v>
       </c>
       <c r="D49">
-        <f>B50-B49</f>
+        <f t="shared" si="3"/>
         <v>-1.9999999999999929</v>
       </c>
       <c r="E49">
-        <f>A50-A49</f>
+        <f t="shared" si="4"/>
         <v>-12</v>
       </c>
       <c r="F49">
-        <f>D49/E49</f>
+        <f t="shared" si="5"/>
         <v>0.16666666666666607</v>
       </c>
     </row>
@@ -17885,15 +18058,15 @@
         <v>62.6</v>
       </c>
       <c r="D50">
-        <f>B51-B50</f>
+        <f t="shared" si="3"/>
         <v>-3.3999999999999986</v>
       </c>
       <c r="E50">
-        <f>A51-A50</f>
+        <f t="shared" si="4"/>
         <v>-16</v>
       </c>
       <c r="F50">
-        <f>D50/E50</f>
+        <f t="shared" si="5"/>
         <v>0.21249999999999991</v>
       </c>
     </row>
@@ -17905,15 +18078,15 @@
         <v>59.2</v>
       </c>
       <c r="D51">
-        <f>B52-B51</f>
+        <f t="shared" si="3"/>
         <v>-18.800000000000004</v>
       </c>
       <c r="E51">
-        <f>A52-A51</f>
+        <f t="shared" si="4"/>
         <v>-14</v>
       </c>
       <c r="F51">
-        <f>D51/E51</f>
+        <f t="shared" si="5"/>
         <v>1.3428571428571432</v>
       </c>
     </row>
@@ -17925,15 +18098,15 @@
         <v>40.4</v>
       </c>
       <c r="D52">
-        <f>B53-B52</f>
+        <f t="shared" si="3"/>
         <v>-7.1000000000000014</v>
       </c>
       <c r="E52">
-        <f>A53-A52</f>
+        <f t="shared" si="4"/>
         <v>-17</v>
       </c>
       <c r="F52">
-        <f>D52/E52</f>
+        <f t="shared" si="5"/>
         <v>0.41764705882352948</v>
       </c>
     </row>
@@ -17945,15 +18118,15 @@
         <v>33.299999999999997</v>
       </c>
       <c r="D53">
-        <f>B54-B53</f>
+        <f t="shared" si="3"/>
         <v>-4.1999999999999957</v>
       </c>
       <c r="E53">
-        <f>A54-A53</f>
+        <f t="shared" si="4"/>
         <v>-11</v>
       </c>
       <c r="F53">
-        <f>D53/E53</f>
+        <f t="shared" si="5"/>
         <v>0.38181818181818145</v>
       </c>
     </row>
@@ -17965,15 +18138,15 @@
         <v>29.1</v>
       </c>
       <c r="D54">
-        <f>B55-B54</f>
+        <f t="shared" si="3"/>
         <v>-3.1000000000000014</v>
       </c>
       <c r="E54">
-        <f>A55-A54</f>
+        <f t="shared" si="4"/>
         <v>-8</v>
       </c>
       <c r="F54">
-        <f>D54/E54</f>
+        <f t="shared" si="5"/>
         <v>0.38750000000000018</v>
       </c>
     </row>
@@ -17985,15 +18158,15 @@
         <v>26</v>
       </c>
       <c r="D55">
-        <f>B56-B55</f>
+        <f t="shared" si="3"/>
         <v>-1.6000000000000014</v>
       </c>
       <c r="E55">
-        <f>A56-A55</f>
+        <f t="shared" si="4"/>
         <v>-6</v>
       </c>
       <c r="F55">
-        <f>D55/E55</f>
+        <f t="shared" si="5"/>
         <v>0.26666666666666689</v>
       </c>
     </row>
@@ -18008,15 +18181,15 @@
         <v>10</v>
       </c>
       <c r="D56">
-        <f>B57-B56</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E56">
-        <f>A57-A56</f>
+        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
       <c r="F56">
-        <f>D56/E56</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -18028,15 +18201,15 @@
         <v>24.4</v>
       </c>
       <c r="D57">
-        <f>B58-B57</f>
+        <f t="shared" si="3"/>
         <v>0.20000000000000284</v>
       </c>
       <c r="E57">
-        <f>A58-A57</f>
+        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
       <c r="F57">
-        <f>D57/E57</f>
+        <f t="shared" si="5"/>
         <v>-4.000000000000057E-2</v>
       </c>
     </row>
@@ -18056,7 +18229,7 @@
         <v>0</v>
       </c>
       <c r="F58" t="e">
-        <f>D58/E58</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -18073,8 +18246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0713DE22-F4B5-4D13-83A7-330501B9228B}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>